<commit_message>
code without mp.Manager() and queue seems to work as well - time however 5.7min for 100 sim...
</commit_message>
<xml_diff>
--- a/PhaseResults/PhaseFive.xlsx
+++ b/PhaseResults/PhaseFive.xlsx
@@ -468,46 +468,46 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-0.7910919035567063</v>
+        <v>-20.60755986554534</v>
       </c>
       <c r="C2">
-        <v>50.41206673697857</v>
+        <v>1.089226581658092</v>
       </c>
       <c r="D2">
-        <v>-94.26830818621607</v>
+        <v>75.00302793421463</v>
       </c>
       <c r="E2">
-        <v>6.401594338606838</v>
+        <v>-0.406779944259445</v>
       </c>
       <c r="F2">
-        <v>0.7933170358247228</v>
+        <v>-0.352054911594391</v>
       </c>
       <c r="G2">
-        <v>-1.486439936742265</v>
+        <v>0.7815408847023604</v>
       </c>
       <c r="H2">
-        <v>0.1079615911618466</v>
+        <v>-0.4500861918092851</v>
       </c>
       <c r="I2">
-        <v>0.5572170276550641</v>
+        <v>0.8988809271980212</v>
       </c>
       <c r="J2">
-        <v>4.35527313958724</v>
+        <v>4.3552525155391</v>
       </c>
       <c r="K2">
-        <v>88</v>
+        <v>27</v>
       </c>
       <c r="L2">
-        <v>108.7444543868428</v>
+        <v>-13.08276063154555</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>4.355273139587325</v>
+        <v>4.35525251498856</v>
       </c>
       <c r="O2">
-        <v>5.021939806253992</v>
+        <v>5.021919181655227</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -515,46 +515,46 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-2.588492742287783</v>
+        <v>6.489415692342842e-06</v>
       </c>
       <c r="C3">
-        <v>59.4955417929889</v>
+        <v>0.7035650081437954</v>
       </c>
       <c r="D3">
-        <v>-0.1206105271962045</v>
+        <v>1.195271404766907</v>
       </c>
       <c r="E3">
-        <v>0.8991852839758899</v>
+        <v>62.69770586818203</v>
       </c>
       <c r="F3">
-        <v>0.469548705034859</v>
+        <v>1.653471968311442</v>
       </c>
       <c r="G3">
-        <v>-0.8691388670716602</v>
+        <v>-1.727242461161577</v>
       </c>
       <c r="H3">
-        <v>1.088230191009552</v>
+        <v>0.5345901828952315</v>
       </c>
       <c r="I3">
-        <v>0.8422309730537911</v>
+        <v>-0.6299647063015685</v>
       </c>
       <c r="J3">
-        <v>4.355294202799492</v>
+        <v>4.355350724842692</v>
       </c>
       <c r="K3">
-        <v>14</v>
+        <v>98</v>
       </c>
       <c r="L3">
-        <v>2.614780721703519</v>
+        <v>-10.91721351340661</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3">
-        <v>4.355294202798172</v>
+        <v>4.355350721035633</v>
       </c>
       <c r="O3">
-        <v>5.021960869464839</v>
+        <v>5.0220173877023</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -562,46 +562,46 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>9.425927177164892</v>
+        <v>-1.836450284879223</v>
       </c>
       <c r="C4">
-        <v>-45.60704779270113</v>
+        <v>62.8767700094226</v>
       </c>
       <c r="D4">
-        <v>84.2291156520397</v>
+        <v>0.1799469150252427</v>
       </c>
       <c r="E4">
-        <v>0.1214625541539565</v>
+        <v>-0.0001415292567473507</v>
       </c>
       <c r="F4">
-        <v>0.150877507450629</v>
+        <v>-0.6433970046019519</v>
       </c>
       <c r="G4">
-        <v>-0.105701273238999</v>
+        <v>-0.7616181374878477</v>
       </c>
       <c r="H4">
-        <v>-0.4725403536080177</v>
+        <v>0.8604019339048006</v>
       </c>
       <c r="I4">
-        <v>0.8087446480601739</v>
+        <v>1.848922505396178</v>
       </c>
       <c r="J4">
-        <v>4.355354434053086</v>
+        <v>4.355362752407631</v>
       </c>
       <c r="K4">
-        <v>99</v>
+        <v>17</v>
       </c>
       <c r="L4">
-        <v>1.112879480791088</v>
+        <v>-3.972176334657421</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
-        <v>4.355354434053088</v>
+        <v>4.35536275239051</v>
       </c>
       <c r="O4">
-        <v>5.022021100719755</v>
+        <v>5.022029419057177</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -609,46 +609,46 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>22.42637501791641</v>
+        <v>0.3725194491593553</v>
       </c>
       <c r="C5">
-        <v>-0.8448602280351153</v>
+        <v>8.517556335889296</v>
       </c>
       <c r="D5">
-        <v>1.015474669054758</v>
+        <v>58.72967226374491</v>
       </c>
       <c r="E5">
-        <v>56.03970426068496</v>
+        <v>-0.0290272403757472</v>
       </c>
       <c r="F5">
-        <v>-0.4812570140536239</v>
+        <v>0.7927274845000563</v>
       </c>
       <c r="G5">
-        <v>1.067095122165743</v>
+        <v>-1.324838884042288</v>
       </c>
       <c r="H5">
-        <v>1.043915563622367</v>
+        <v>-0.7077263909663822</v>
       </c>
       <c r="I5">
-        <v>-1.080361874907176</v>
+        <v>1.073934080018848</v>
       </c>
       <c r="J5">
-        <v>4.355381844038249</v>
+        <v>4.355367582331654</v>
       </c>
       <c r="K5">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="L5">
-        <v>-5.503620951881429</v>
+        <v>-5.976831165322857</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5">
-        <v>4.355381844056252</v>
+        <v>4.355367582335208</v>
       </c>
       <c r="O5">
-        <v>5.022048510722919</v>
+        <v>5.022034249001875</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -656,46 +656,46 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>23.71388405557948</v>
+        <v>-0.3630679222453754</v>
       </c>
       <c r="C6">
-        <v>45.61443794615744</v>
+        <v>1.444344719566855</v>
       </c>
       <c r="D6">
-        <v>-34.12200972406686</v>
+        <v>47.84348870804013</v>
       </c>
       <c r="E6">
-        <v>44.17163785833594</v>
+        <v>20.08156574257011</v>
       </c>
       <c r="F6">
-        <v>0.288537142158857</v>
+        <v>0.8703964381228366</v>
       </c>
       <c r="G6">
-        <v>-0.1888115580793215</v>
+        <v>0.7040910487935337</v>
       </c>
       <c r="H6">
-        <v>0.1956073232816409</v>
+        <v>-0.3947333488908169</v>
       </c>
       <c r="I6">
-        <v>-1.01714007460956</v>
+        <v>-0.8932278747492548</v>
       </c>
       <c r="J6">
-        <v>4.354231060773191</v>
+        <v>4.354054096912488</v>
       </c>
       <c r="K6">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="L6">
-        <v>-18.49301368400148</v>
+        <v>-18.49099562563747</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6">
-        <v>4.355450999467294</v>
+        <v>4.355476733141792</v>
       </c>
       <c r="O6">
-        <v>5.022117666133961</v>
+        <v>5.022143399808459</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit for branch change
</commit_message>
<xml_diff>
--- a/PhaseResults/PhaseFive.xlsx
+++ b/PhaseResults/PhaseFive.xlsx
@@ -468,46 +468,46 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-20.60755986554534</v>
+        <v>0.512427745349363</v>
       </c>
       <c r="C2">
-        <v>1.089226581658092</v>
+        <v>-1.363767227788882</v>
       </c>
       <c r="D2">
-        <v>75.00302793421463</v>
+        <v>59.70675209903689</v>
       </c>
       <c r="E2">
-        <v>-0.406779944259445</v>
+        <v>-0.0003999063564507079</v>
       </c>
       <c r="F2">
-        <v>-0.352054911594391</v>
+        <v>0.6898044308789899</v>
       </c>
       <c r="G2">
-        <v>0.7815408847023604</v>
+        <v>-0.5004414916667799</v>
       </c>
       <c r="H2">
-        <v>-0.4500861918092851</v>
+        <v>-0.6350004731026235</v>
       </c>
       <c r="I2">
-        <v>0.8988809271980212</v>
+        <v>1.621664813878342</v>
       </c>
       <c r="J2">
-        <v>4.3552525155391</v>
+        <v>4.355285082868471</v>
       </c>
       <c r="K2">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="L2">
-        <v>-13.08276063154555</v>
+        <v>-8.080333650738645</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>4.35525251498856</v>
+        <v>4.355285082866482</v>
       </c>
       <c r="O2">
-        <v>5.021919181655227</v>
+        <v>5.021951749533149</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -515,46 +515,46 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>6.489415692342842e-06</v>
+        <v>6.780578827585828</v>
       </c>
       <c r="C3">
-        <v>0.7035650081437954</v>
+        <v>53.10279935400346</v>
       </c>
       <c r="D3">
-        <v>1.195271404766907</v>
+        <v>-89.19799699470447</v>
       </c>
       <c r="E3">
-        <v>62.69770586818203</v>
+        <v>-5.418064916170746e-05</v>
       </c>
       <c r="F3">
-        <v>1.653471968311442</v>
+        <v>0.37163061194269</v>
       </c>
       <c r="G3">
-        <v>-1.727242461161577</v>
+        <v>-0.3368040805509991</v>
       </c>
       <c r="H3">
-        <v>0.5345901828952315</v>
+        <v>0.0386712405137799</v>
       </c>
       <c r="I3">
-        <v>-0.6299647063015685</v>
+        <v>1.890841099281444</v>
       </c>
       <c r="J3">
-        <v>4.355350724842692</v>
+        <v>4.355295902663592</v>
       </c>
       <c r="K3">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="L3">
-        <v>-10.91721351340661</v>
+        <v>64.70060460020855</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3">
-        <v>4.355350721035633</v>
+        <v>4.355295902660338</v>
       </c>
       <c r="O3">
-        <v>5.0220173877023</v>
+        <v>5.021962569327004</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -562,46 +562,46 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-1.836450284879223</v>
+        <v>-0.01513397410389549</v>
       </c>
       <c r="C4">
-        <v>62.8767700094226</v>
+        <v>25.15261976488516</v>
       </c>
       <c r="D4">
-        <v>0.1799469150252427</v>
+        <v>44.35061839695146</v>
       </c>
       <c r="E4">
-        <v>-0.0001415292567473507</v>
+        <v>0.2877657036915104</v>
       </c>
       <c r="F4">
-        <v>-0.6433970046019519</v>
+        <v>1.18443800501441</v>
       </c>
       <c r="G4">
-        <v>-0.7616181374878477</v>
+        <v>-0.5605967116354871</v>
       </c>
       <c r="H4">
-        <v>0.8604019339048006</v>
+        <v>-0.9456454821981288</v>
       </c>
       <c r="I4">
-        <v>1.848922505396178</v>
+        <v>0.8338599972250136</v>
       </c>
       <c r="J4">
-        <v>4.355362752407631</v>
+        <v>4.355369250924604</v>
       </c>
       <c r="K4">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="L4">
-        <v>-3.972176334657421</v>
+        <v>-5.761773861116499</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
-        <v>4.35536275239051</v>
+        <v>4.355369250931052</v>
       </c>
       <c r="O4">
-        <v>5.022029419057177</v>
+        <v>5.022035917597719</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -609,46 +609,46 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.3725194491593553</v>
+        <v>5.379649467481933</v>
       </c>
       <c r="C5">
-        <v>8.517556335889296</v>
+        <v>-2.599789483648555</v>
       </c>
       <c r="D5">
-        <v>58.72967226374491</v>
+        <v>20.55006959486832</v>
       </c>
       <c r="E5">
-        <v>-0.0290272403757472</v>
+        <v>50.21933496961683</v>
       </c>
       <c r="F5">
-        <v>0.7927274845000563</v>
+        <v>0.5961330041681703</v>
       </c>
       <c r="G5">
-        <v>-1.324838884042288</v>
+        <v>0.6765836970136485</v>
       </c>
       <c r="H5">
-        <v>-0.7077263909663822</v>
+        <v>-0.3212336317668543</v>
       </c>
       <c r="I5">
-        <v>1.073934080018848</v>
+        <v>-0.3538195067581045</v>
       </c>
       <c r="J5">
-        <v>4.355367582331654</v>
+        <v>4.354102017697073</v>
       </c>
       <c r="K5">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="L5">
-        <v>-5.976831165322857</v>
+        <v>-33.0665014051261</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5">
-        <v>4.355367582335208</v>
+        <v>4.355385754896673</v>
       </c>
       <c r="O5">
-        <v>5.022034249001875</v>
+        <v>5.02205242156334</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -656,46 +656,46 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>-0.3630679222453754</v>
+        <v>-18.14343379251174</v>
       </c>
       <c r="C6">
-        <v>1.444344719566855</v>
+        <v>49.29212575291513</v>
       </c>
       <c r="D6">
-        <v>47.84348870804013</v>
+        <v>1.855967475239631</v>
       </c>
       <c r="E6">
-        <v>20.08156574257011</v>
+        <v>31.11628356901486</v>
       </c>
       <c r="F6">
-        <v>0.8703964381228366</v>
+        <v>-0.6542334917483561</v>
       </c>
       <c r="G6">
-        <v>0.7040910487935337</v>
+        <v>-0.6422895521552101</v>
       </c>
       <c r="H6">
-        <v>-0.3947333488908169</v>
+        <v>0.489667206518646</v>
       </c>
       <c r="I6">
-        <v>-0.8932278747492548</v>
+        <v>-0.3677553154227562</v>
       </c>
       <c r="J6">
-        <v>4.354054096912488</v>
+        <v>4.354322482717333</v>
       </c>
       <c r="K6">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="L6">
-        <v>-18.49099562563747</v>
+        <v>-18.49407682031511</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6">
-        <v>4.355476733141792</v>
+        <v>4.355388030443549</v>
       </c>
       <c r="O6">
-        <v>5.022143399808459</v>
+        <v>5.022054697110216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>